<commit_message>
Assignment completed up to task 12
</commit_message>
<xml_diff>
--- a/591528am_NA1.xlsx
+++ b/591528am_NA1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreamontalto/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreamontalto/Desktop/Github/DMA/Assignment_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B326FBC-C712-624B-92DC-F9DF9D4F83A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AF4879-D6AD-604A-85EE-E89E020840AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{B7FF788D-1D64-4368-BFD3-4AAB7F5CE5F9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{B7FF788D-1D64-4368-BFD3-4AAB7F5CE5F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>question</t>
   </si>
@@ -45,6 +45,18 @@
   </si>
   <si>
     <t>12B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x7 </t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -80,8 +92,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,7 +412,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -419,55 +432,88 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>0.14099999999999999</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>0.93700000000000006</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>4.0400000000000002E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>3.3700000000000002E-3</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" s="1">
+        <v>26.7</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>